<commit_message>
Fix some typos and update info
</commit_message>
<xml_diff>
--- a/COA/coa_Choi_2020_Sep.xlsx
+++ b/COA/coa_Choi_2020_Sep.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8351533-9B47-2044-8AD0-38C32D1B30E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739417DA-5C05-5A4E-AA07-FB7658536DDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15360" yWindow="1560" windowWidth="26940" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="348">
   <si>
     <t>G:</t>
   </si>
@@ -397,9 +397,6 @@
     <t>Computer Science</t>
   </si>
   <si>
-    <t>Misericordia University</t>
-  </si>
-  <si>
     <t xml:space="preserve">Larsen, Rasmus Munk </t>
   </si>
   <si>
@@ -458,9 +455,6 @@
   </si>
   <si>
     <t>lluisantoni@gmail.com</t>
-  </si>
-  <si>
-    <t>Hyatt Hotels Corporation</t>
   </si>
   <si>
     <t>lanjiang61930@gmail.com</t>
@@ -1148,24 +1142,15 @@
     <t>ishaoranwang@gmail.com</t>
   </si>
   <si>
-    <t>SigOpts Inc.</t>
-  </si>
-  <si>
     <t>mccourt@sigopt.com</t>
   </si>
   <si>
-    <t>Victor Wu</t>
-  </si>
-  <si>
     <t>wu.victor@gmail.com</t>
   </si>
   <si>
     <t>Tilt Dev Computer Software</t>
   </si>
   <si>
-    <t>Jonathan Ashbeck</t>
-  </si>
-  <si>
     <t>jashbeck@sas.upenn.edu</t>
   </si>
   <si>
@@ -1227,6 +1212,18 @@
   </si>
   <si>
     <t>RJarrow@kamakuraco.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wu, Victor </t>
+  </si>
+  <si>
+    <t>Ashbeck, Jonathan</t>
+  </si>
+  <si>
+    <t>Compass</t>
+  </si>
+  <si>
+    <t>SigOpt, Inc.</t>
   </si>
 </sst>
 </file>
@@ -1504,7 +1501,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -1737,10 +1734,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -1794,6 +1787,18 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2960,7 +2965,9 @@
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="TableD5" displayName="TableD5" ref="A187:E211" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="A187:E211" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A188:E211">
+    <sortCondition ref="B188:B211"/>
+  </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="5" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name:" dataDxfId="12"/>
@@ -3206,14 +3213,14 @@
   </sheetPr>
   <dimension ref="A1:R211"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A162" zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="C175" sqref="C175"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A148" zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="D157" sqref="D157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.19921875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.19921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="34.59765625" style="1" customWidth="1"/>
     <col min="4" max="4" width="47.3984375" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.3984375" style="1" customWidth="1"/>
@@ -3225,137 +3232,137 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="195.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
     </row>
     <row r="2" spans="1:5" s="9" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
     </row>
     <row r="3" spans="1:5" s="9" customFormat="1" ht="67.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
     </row>
     <row r="4" spans="1:5" s="9" customFormat="1" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
     </row>
     <row r="5" spans="1:5" s="9" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
     </row>
     <row r="6" spans="1:5" s="9" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="84" t="s">
+      <c r="A6" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
     </row>
     <row r="7" spans="1:5" s="10" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="85" t="s">
+      <c r="A7" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
+      <c r="B7" s="84"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
     </row>
     <row r="8" spans="1:5" ht="62.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="85" t="s">
+      <c r="A8" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="85"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="84"/>
     </row>
     <row r="9" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="85" t="s">
+      <c r="A9" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="85"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
+      <c r="B9" s="84"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="84"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="85" t="s">
+      <c r="A10" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="85"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="85" t="s">
+      <c r="A11" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="85"/>
-      <c r="C11" s="85"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="85"/>
+      <c r="B11" s="84"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
     </row>
     <row r="12" spans="1:5" s="5" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="89" t="s">
+      <c r="A12" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="90"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="90"/>
-      <c r="E12" s="90"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="89"/>
     </row>
     <row r="13" spans="1:5" s="9" customFormat="1" ht="49.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="85" t="s">
+      <c r="A13" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="85"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="84"/>
     </row>
     <row r="14" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="87"/>
-      <c r="B14" s="87"/>
-      <c r="C14" s="87"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="87"/>
+      <c r="A14" s="86"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
     </row>
     <row r="15" spans="1:5" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="86" t="s">
+      <c r="A15" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="85"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="35" t="s">
@@ -3406,16 +3413,16 @@
       <c r="C19" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="81">
+      <c r="D19" s="80">
         <v>43861</v>
       </c>
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="39"/>
-      <c r="B20" s="82"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="81"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="80"/>
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" s="12" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3429,24 +3436,24 @@
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="86" t="s">
+      <c r="A23" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="86"/>
-      <c r="C23" s="86"/>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="85"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
     </row>
     <row r="24" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="91" t="s">
+      <c r="B24" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="91"/>
-      <c r="D24" s="91"/>
-      <c r="E24" s="91"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="90"/>
+      <c r="E24" s="90"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
@@ -3525,24 +3532,24 @@
       <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:5" s="5" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="86" t="s">
+      <c r="A33" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="86"/>
-      <c r="C33" s="86"/>
-      <c r="D33" s="86"/>
-      <c r="E33" s="86"/>
+      <c r="B33" s="85"/>
+      <c r="C33" s="85"/>
+      <c r="D33" s="85"/>
+      <c r="E33" s="85"/>
     </row>
     <row r="34" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="83" t="s">
+      <c r="B34" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="83"/>
-      <c r="D34" s="83"/>
-      <c r="E34" s="83"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="82"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
@@ -3576,7 +3583,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="76" t="s">
+      <c r="A38" s="75" t="s">
         <v>0</v>
       </c>
       <c r="B38" s="40" t="s">
@@ -3590,7 +3597,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="76" t="s">
+      <c r="A39" s="75" t="s">
         <v>0</v>
       </c>
       <c r="B39" s="40" t="s">
@@ -3604,47 +3611,47 @@
       </c>
     </row>
     <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="76" t="s">
+      <c r="A40" s="75" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="40" t="s">
+      <c r="D40" s="43"/>
+    </row>
+    <row r="41" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="D40" s="43"/>
-    </row>
-    <row r="41" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="76" t="s">
+      <c r="C41" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="43" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="D41" s="43" t="s">
+      <c r="B42" s="40" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="76" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="40" t="s">
-        <v>78</v>
       </c>
       <c r="C42" s="40" t="s">
         <v>57</v>
       </c>
       <c r="D42" s="43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="76" t="s">
+      <c r="A43" s="75" t="s">
         <v>2</v>
       </c>
       <c r="B43" s="40" t="s">
@@ -3653,8 +3660,8 @@
       <c r="C43" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="80" t="s">
-        <v>332</v>
+      <c r="D43" s="79" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3755,24 +3762,24 @@
       <c r="E59" s="4"/>
     </row>
     <row r="60" spans="1:5" s="2" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="86" t="s">
+      <c r="A60" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="B60" s="86"/>
-      <c r="C60" s="86"/>
-      <c r="D60" s="86"/>
-      <c r="E60" s="86"/>
+      <c r="B60" s="85"/>
+      <c r="C60" s="85"/>
+      <c r="D60" s="85"/>
+      <c r="E60" s="85"/>
     </row>
     <row r="61" spans="1:5" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B61" s="83" t="s">
+      <c r="B61" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="C61" s="83"/>
-      <c r="D61" s="83"/>
-      <c r="E61" s="83"/>
+      <c r="C61" s="82"/>
+      <c r="D61" s="82"/>
+      <c r="E61" s="82"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="34" t="s">
@@ -3812,7 +3819,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="77" t="s">
+      <c r="A65" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B65" s="50" t="s">
@@ -3829,303 +3836,303 @@
       </c>
     </row>
     <row r="66" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A66" s="77" t="s">
+      <c r="A66" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B66" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="C66" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="D66" s="43" t="s">
         <v>104</v>
-      </c>
-      <c r="C66" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="D66" s="43" t="s">
-        <v>106</v>
       </c>
       <c r="E66" s="48">
         <v>41729</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A67" s="77" t="s">
+      <c r="A67" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B67" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="C67" s="50" t="s">
+        <v>201</v>
+      </c>
+      <c r="D67" s="43" t="s">
         <v>202</v>
-      </c>
-      <c r="C67" s="50" t="s">
-        <v>203</v>
-      </c>
-      <c r="D67" s="43" t="s">
-        <v>204</v>
       </c>
       <c r="E67" s="48">
         <v>41829</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A68" s="77" t="s">
+      <c r="A68" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B68" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="C68" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="D68" s="43" t="s">
         <v>131</v>
-      </c>
-      <c r="C68" s="50" t="s">
-        <v>132</v>
-      </c>
-      <c r="D68" s="43" t="s">
-        <v>133</v>
       </c>
       <c r="E68" s="48">
         <v>41829</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="79" t="s">
+      <c r="A69" s="78" t="s">
         <v>8</v>
       </c>
       <c r="B69" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="C69" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="D69" s="42" t="s">
         <v>137</v>
-      </c>
-      <c r="C69" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="D69" s="42" t="s">
-        <v>139</v>
       </c>
       <c r="E69" s="54">
         <v>41829</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A70" s="77" t="s">
+      <c r="A70" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B70" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="C70" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="D70" s="43" t="s">
         <v>140</v>
-      </c>
-      <c r="C70" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="D70" s="43" t="s">
-        <v>142</v>
       </c>
       <c r="E70" s="48">
         <v>41829</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A71" s="77" t="s">
+      <c r="A71" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B71" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="C71" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="D71" s="43" t="s">
         <v>128</v>
-      </c>
-      <c r="C71" s="40" t="s">
-        <v>129</v>
-      </c>
-      <c r="D71" s="43" t="s">
-        <v>130</v>
       </c>
       <c r="E71" s="48">
         <v>41829</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A72" s="77" t="s">
+      <c r="A72" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B72" s="64" t="s">
+        <v>197</v>
+      </c>
+      <c r="C72" s="64" t="s">
+        <v>198</v>
+      </c>
+      <c r="D72" s="43" t="s">
         <v>199</v>
-      </c>
-      <c r="C72" s="64" t="s">
-        <v>200</v>
-      </c>
-      <c r="D72" s="43" t="s">
-        <v>201</v>
       </c>
       <c r="E72" s="48">
         <v>41829</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A73" s="77" t="s">
+      <c r="A73" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B73" s="40" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C73" s="40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D73" s="43" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E73" s="48">
         <v>41829</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A74" s="77" t="s">
+      <c r="A74" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B74" s="50" t="s">
+        <v>191</v>
+      </c>
+      <c r="C74" s="50" t="s">
+        <v>192</v>
+      </c>
+      <c r="D74" s="43" t="s">
         <v>193</v>
-      </c>
-      <c r="C74" s="50" t="s">
-        <v>194</v>
-      </c>
-      <c r="D74" s="43" t="s">
-        <v>195</v>
       </c>
       <c r="E74" s="48">
         <v>42422</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A75" s="77" t="s">
+      <c r="A75" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B75" s="50" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C75" s="50" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D75" s="45" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E75" s="48">
         <v>42422</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A76" s="77" t="s">
+      <c r="A76" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B76" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="C76" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="D76" s="43" t="s">
         <v>184</v>
-      </c>
-      <c r="C76" s="50" t="s">
-        <v>185</v>
-      </c>
-      <c r="D76" s="43" t="s">
-        <v>186</v>
       </c>
       <c r="E76" s="48">
         <v>42422</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A77" s="77" t="s">
+      <c r="A77" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B77" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C77" s="50" t="s">
+        <v>133</v>
+      </c>
+      <c r="D77" s="43" t="s">
         <v>134</v>
-      </c>
-      <c r="C77" s="50" t="s">
-        <v>135</v>
-      </c>
-      <c r="D77" s="43" t="s">
-        <v>136</v>
       </c>
       <c r="E77" s="48">
         <v>42422</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A78" s="77" t="s">
+      <c r="A78" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B78" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="C78" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="D78" s="45" t="s">
         <v>190</v>
-      </c>
-      <c r="C78" s="50" t="s">
-        <v>191</v>
-      </c>
-      <c r="D78" s="45" t="s">
-        <v>192</v>
       </c>
       <c r="E78" s="48">
         <v>42422</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A79" s="77" t="s">
+      <c r="A79" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B79" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="C79" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="D79" s="43" t="s">
         <v>196</v>
-      </c>
-      <c r="C79" s="50" t="s">
-        <v>197</v>
-      </c>
-      <c r="D79" s="43" t="s">
-        <v>198</v>
       </c>
       <c r="E79" s="48">
         <v>42422</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A80" s="77" t="s">
+      <c r="A80" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B80" s="49" t="s">
+        <v>185</v>
+      </c>
+      <c r="C80" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="D80" s="51" t="s">
         <v>187</v>
-      </c>
-      <c r="C80" s="50" t="s">
-        <v>188</v>
-      </c>
-      <c r="D80" s="51" t="s">
-        <v>189</v>
       </c>
       <c r="E80" s="48">
         <v>42422</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A81" s="77" t="s">
+      <c r="A81" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B81" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="C81" s="49" t="s">
+        <v>109</v>
+      </c>
+      <c r="D81" s="73" t="s">
         <v>110</v>
-      </c>
-      <c r="C81" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="D81" s="73" t="s">
-        <v>112</v>
       </c>
       <c r="E81" s="48">
         <v>42422</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A82" s="77" t="s">
+      <c r="A82" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B82" s="50" t="s">
+        <v>221</v>
+      </c>
+      <c r="C82" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="D82" s="45" t="s">
         <v>223</v>
-      </c>
-      <c r="C82" s="50" t="s">
-        <v>224</v>
-      </c>
-      <c r="D82" s="45" t="s">
-        <v>225</v>
       </c>
       <c r="E82" s="48">
         <v>42632</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A83" s="77" t="s">
+      <c r="A83" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B83" s="53" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C83" s="53" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D83" s="56"/>
       <c r="E83" s="48">
@@ -4133,14 +4140,14 @@
       </c>
     </row>
     <row r="84" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A84" s="77" t="s">
+      <c r="A84" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B84" s="53" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C84" s="53" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D84" s="56"/>
       <c r="E84" s="48">
@@ -4148,14 +4155,14 @@
       </c>
     </row>
     <row r="85" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A85" s="77" t="s">
+      <c r="A85" s="76" t="s">
         <v>8</v>
       </c>
       <c r="B85" s="53" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C85" s="53" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D85" s="56"/>
       <c r="E85" s="48">
@@ -4163,14 +4170,14 @@
       </c>
     </row>
     <row r="86" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A86" s="78" t="s">
+      <c r="A86" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B86" s="50" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C86" s="50" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D86" s="45"/>
       <c r="E86" s="48">
@@ -4178,14 +4185,14 @@
       </c>
     </row>
     <row r="87" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A87" s="78" t="s">
+      <c r="A87" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B87" s="50" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C87" s="50" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D87" s="45"/>
       <c r="E87" s="48">
@@ -4193,14 +4200,14 @@
       </c>
     </row>
     <row r="88" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A88" s="78" t="s">
+      <c r="A88" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B88" s="50" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C88" s="50" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D88" s="45"/>
       <c r="E88" s="48">
@@ -4208,65 +4215,65 @@
       </c>
     </row>
     <row r="89" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A89" s="78" t="s">
+      <c r="A89" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B89" s="50" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C89" s="59" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D89" s="45" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E89" s="48">
         <v>42632</v>
       </c>
     </row>
     <row r="90" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A90" s="78" t="s">
+      <c r="A90" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B90" s="50" t="s">
+        <v>237</v>
+      </c>
+      <c r="C90" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="D90" s="45" t="s">
         <v>239</v>
-      </c>
-      <c r="C90" s="59" t="s">
-        <v>240</v>
-      </c>
-      <c r="D90" s="45" t="s">
-        <v>241</v>
       </c>
       <c r="E90" s="48">
         <v>42632</v>
       </c>
     </row>
     <row r="91" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A91" s="78" t="s">
+      <c r="A91" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B91" s="50" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C91" s="59" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D91" s="45" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E91" s="48">
         <v>42632</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A92" s="78" t="s">
+      <c r="A92" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B92" s="49" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C92" s="62" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D92" s="49"/>
       <c r="E92" s="48">
@@ -4274,14 +4281,14 @@
       </c>
     </row>
     <row r="93" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A93" s="78" t="s">
+      <c r="A93" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B93" s="50" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C93" s="59" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D93" s="45"/>
       <c r="E93" s="48">
@@ -4289,65 +4296,65 @@
       </c>
     </row>
     <row r="94" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A94" s="78" t="s">
+      <c r="A94" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B94" s="50" t="s">
+        <v>245</v>
+      </c>
+      <c r="C94" s="59" t="s">
+        <v>246</v>
+      </c>
+      <c r="D94" s="45" t="s">
         <v>247</v>
-      </c>
-      <c r="C94" s="59" t="s">
-        <v>248</v>
-      </c>
-      <c r="D94" s="45" t="s">
-        <v>249</v>
       </c>
       <c r="E94" s="48">
         <v>42632</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A95" s="78" t="s">
+      <c r="A95" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B95" s="50" t="s">
+        <v>248</v>
+      </c>
+      <c r="C95" s="59" t="s">
+        <v>249</v>
+      </c>
+      <c r="D95" s="45" t="s">
         <v>250</v>
-      </c>
-      <c r="C95" s="59" t="s">
-        <v>251</v>
-      </c>
-      <c r="D95" s="45" t="s">
-        <v>252</v>
       </c>
       <c r="E95" s="48">
         <v>42632</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A96" s="78" t="s">
+      <c r="A96" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B96" s="49" t="s">
+        <v>251</v>
+      </c>
+      <c r="C96" s="62" t="s">
+        <v>252</v>
+      </c>
+      <c r="D96" s="49" t="s">
         <v>253</v>
-      </c>
-      <c r="C96" s="62" t="s">
-        <v>254</v>
-      </c>
-      <c r="D96" s="49" t="s">
-        <v>255</v>
       </c>
       <c r="E96" s="48">
         <v>42632</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A97" s="78" t="s">
+      <c r="A97" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B97" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C97" s="59" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D97" s="45"/>
       <c r="E97" s="48">
@@ -4355,11 +4362,11 @@
       </c>
     </row>
     <row r="98" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A98" s="78" t="s">
+      <c r="A98" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B98" s="50" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C98" s="59"/>
       <c r="D98" s="45"/>
@@ -4368,14 +4375,14 @@
       </c>
     </row>
     <row r="99" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A99" s="78" t="s">
+      <c r="A99" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B99" s="50" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C99" s="59" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D99" s="45"/>
       <c r="E99" s="48">
@@ -4383,31 +4390,31 @@
       </c>
     </row>
     <row r="100" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A100" s="78" t="s">
+      <c r="A100" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B100" s="50" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C100" s="59" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D100" s="45" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E100" s="48">
         <v>42632</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A101" s="78" t="s">
+      <c r="A101" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B101" s="50" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C101" s="59" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D101" s="45"/>
       <c r="E101" s="48">
@@ -4415,14 +4422,14 @@
       </c>
     </row>
     <row r="102" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A102" s="78" t="s">
+      <c r="A102" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B102" s="50" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C102" s="71" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D102" s="45"/>
       <c r="E102" s="48">
@@ -4430,14 +4437,14 @@
       </c>
     </row>
     <row r="103" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A103" s="78" t="s">
+      <c r="A103" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B103" s="50" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C103" s="71" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D103" s="45"/>
       <c r="E103" s="48">
@@ -4445,14 +4452,14 @@
       </c>
     </row>
     <row r="104" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A104" s="78" t="s">
+      <c r="A104" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B104" s="49" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C104" s="62" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D104" s="49"/>
       <c r="E104" s="48">
@@ -4460,14 +4467,14 @@
       </c>
     </row>
     <row r="105" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A105" s="78" t="s">
+      <c r="A105" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B105" s="50" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C105" s="71" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D105" s="45"/>
       <c r="E105" s="48">
@@ -4475,14 +4482,14 @@
       </c>
     </row>
     <row r="106" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A106" s="78" t="s">
+      <c r="A106" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B106" s="50" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C106" s="71" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D106" s="45"/>
       <c r="E106" s="48">
@@ -4490,14 +4497,14 @@
       </c>
     </row>
     <row r="107" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A107" s="78" t="s">
+      <c r="A107" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B107" s="40" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C107" s="63" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D107" s="40"/>
       <c r="E107" s="48">
@@ -4505,14 +4512,14 @@
       </c>
     </row>
     <row r="108" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A108" s="78" t="s">
+      <c r="A108" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B108" s="40" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C108" s="63" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D108" s="40"/>
       <c r="E108" s="48">
@@ -4520,14 +4527,14 @@
       </c>
     </row>
     <row r="109" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="76" t="s">
+      <c r="A109" s="75" t="s">
         <v>8</v>
       </c>
       <c r="B109" s="40" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C109" s="63" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D109" s="40"/>
       <c r="E109" s="54">
@@ -4535,14 +4542,14 @@
       </c>
     </row>
     <row r="110" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A110" s="78" t="s">
+      <c r="A110" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B110" s="40" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C110" s="63" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D110" s="40"/>
       <c r="E110" s="48">
@@ -4550,31 +4557,31 @@
       </c>
     </row>
     <row r="111" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="76" t="s">
+      <c r="A111" s="75" t="s">
         <v>8</v>
       </c>
       <c r="B111" s="40" t="s">
+        <v>278</v>
+      </c>
+      <c r="C111" s="63" t="s">
+        <v>279</v>
+      </c>
+      <c r="D111" s="40" t="s">
         <v>280</v>
-      </c>
-      <c r="C111" s="63" t="s">
-        <v>281</v>
-      </c>
-      <c r="D111" s="40" t="s">
-        <v>282</v>
       </c>
       <c r="E111" s="54">
         <v>42632</v>
       </c>
     </row>
     <row r="112" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A112" s="76" t="s">
+      <c r="A112" s="75" t="s">
         <v>8</v>
       </c>
       <c r="B112" s="40" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C112" s="63" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D112" s="40"/>
       <c r="E112" s="48">
@@ -4582,14 +4589,14 @@
       </c>
     </row>
     <row r="113" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A113" s="76" t="s">
+      <c r="A113" s="75" t="s">
         <v>8</v>
       </c>
       <c r="B113" s="40" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C113" s="72" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D113" s="45"/>
       <c r="E113" s="54">
@@ -4597,14 +4604,14 @@
       </c>
     </row>
     <row r="114" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A114" s="78" t="s">
+      <c r="A114" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B114" s="40" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C114" s="63" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D114" s="45"/>
       <c r="E114" s="48">
@@ -4612,14 +4619,14 @@
       </c>
     </row>
     <row r="115" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A115" s="78" t="s">
+      <c r="A115" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B115" s="40" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C115" s="63" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D115" s="40"/>
       <c r="E115" s="48">
@@ -4627,14 +4634,14 @@
       </c>
     </row>
     <row r="116" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A116" s="78" t="s">
+      <c r="A116" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B116" s="40" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C116" s="63" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D116" s="45"/>
       <c r="E116" s="48">
@@ -4642,14 +4649,14 @@
       </c>
     </row>
     <row r="117" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A117" s="76" t="s">
+      <c r="A117" s="75" t="s">
         <v>8</v>
       </c>
       <c r="B117" s="40" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C117" s="63" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D117" s="40"/>
       <c r="E117" s="48">
@@ -4657,14 +4664,14 @@
       </c>
     </row>
     <row r="118" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="76" t="s">
+      <c r="A118" s="75" t="s">
         <v>8</v>
       </c>
       <c r="B118" s="40" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C118" s="63" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D118" s="40"/>
       <c r="E118" s="54">
@@ -4672,31 +4679,31 @@
       </c>
     </row>
     <row r="119" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A119" s="78" t="s">
+      <c r="A119" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B119" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="C119" s="59" t="s">
+        <v>142</v>
+      </c>
+      <c r="D119" s="45" t="s">
         <v>143</v>
-      </c>
-      <c r="C119" s="59" t="s">
-        <v>144</v>
-      </c>
-      <c r="D119" s="45" t="s">
-        <v>145</v>
       </c>
       <c r="E119" s="48">
         <v>42632</v>
       </c>
     </row>
     <row r="120" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A120" s="78" t="s">
+      <c r="A120" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B120" s="50" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C120" s="71" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D120" s="45"/>
       <c r="E120" s="48">
@@ -4704,14 +4711,14 @@
       </c>
     </row>
     <row r="121" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A121" s="78" t="s">
+      <c r="A121" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B121" s="40" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C121" s="63" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D121" s="45"/>
       <c r="E121" s="48">
@@ -4719,14 +4726,14 @@
       </c>
     </row>
     <row r="122" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A122" s="78" t="s">
+      <c r="A122" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B122" s="40" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C122" s="63" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D122" s="40"/>
       <c r="E122" s="48">
@@ -4734,14 +4741,14 @@
       </c>
     </row>
     <row r="123" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A123" s="76" t="s">
+      <c r="A123" s="75" t="s">
         <v>8</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C123" s="63" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D123" s="40"/>
       <c r="E123" s="48">
@@ -4749,347 +4756,347 @@
       </c>
     </row>
     <row r="124" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A124" s="78" t="s">
+      <c r="A124" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B124" s="50" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C124" s="71" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D124" s="45" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E124" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="125" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A125" s="78" t="s">
+      <c r="A125" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B125" s="50" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C125" s="59" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D125" s="45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E125" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="126" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A126" s="76" t="s">
+      <c r="A126" s="75" t="s">
         <v>8</v>
       </c>
       <c r="B126" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="C126" s="63" t="s">
+        <v>172</v>
+      </c>
+      <c r="D126" s="40" t="s">
         <v>173</v>
-      </c>
-      <c r="C126" s="63" t="s">
-        <v>174</v>
-      </c>
-      <c r="D126" s="40" t="s">
-        <v>175</v>
       </c>
       <c r="E126" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="127" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A127" s="78" t="s">
+      <c r="A127" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B127" s="50" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C127" s="71" t="s">
         <v>58</v>
       </c>
       <c r="D127" s="45" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E127" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="128" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A128" s="78" t="s">
+      <c r="A128" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B128" s="50" t="s">
+        <v>156</v>
+      </c>
+      <c r="C128" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="D128" s="45" t="s">
         <v>158</v>
-      </c>
-      <c r="C128" s="59" t="s">
-        <v>159</v>
-      </c>
-      <c r="D128" s="45" t="s">
-        <v>160</v>
       </c>
       <c r="E128" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="129" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A129" s="78" t="s">
+      <c r="A129" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B129" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="C129" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="D129" s="45" t="s">
         <v>148</v>
-      </c>
-      <c r="C129" s="59" t="s">
-        <v>149</v>
-      </c>
-      <c r="D129" s="45" t="s">
-        <v>150</v>
       </c>
       <c r="E129" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="130" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A130" s="78" t="s">
+      <c r="A130" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B130" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="C130" s="71" t="s">
+        <v>120</v>
+      </c>
+      <c r="D130" s="45" t="s">
         <v>121</v>
-      </c>
-      <c r="C130" s="71" t="s">
-        <v>122</v>
-      </c>
-      <c r="D130" s="45" t="s">
-        <v>123</v>
       </c>
       <c r="E130" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="131" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A131" s="78" t="s">
+      <c r="A131" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B131" s="50" t="s">
+        <v>174</v>
+      </c>
+      <c r="C131" s="59" t="s">
+        <v>175</v>
+      </c>
+      <c r="D131" s="45" t="s">
         <v>176</v>
-      </c>
-      <c r="C131" s="59" t="s">
-        <v>177</v>
-      </c>
-      <c r="D131" s="45" t="s">
-        <v>178</v>
       </c>
       <c r="E131" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="132" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A132" s="78" t="s">
+      <c r="A132" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B132" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="C132" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="D132" s="45" t="s">
         <v>151</v>
-      </c>
-      <c r="C132" s="59" t="s">
-        <v>152</v>
-      </c>
-      <c r="D132" s="45" t="s">
-        <v>153</v>
       </c>
       <c r="E132" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="133" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A133" s="78" t="s">
+      <c r="A133" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B133" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="C133" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="D133" s="45" t="s">
         <v>161</v>
-      </c>
-      <c r="C133" s="59" t="s">
-        <v>162</v>
-      </c>
-      <c r="D133" s="45" t="s">
-        <v>163</v>
       </c>
       <c r="E133" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="134" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A134" s="78" t="s">
+      <c r="A134" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B134" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="C134" s="71" t="s">
         <v>80</v>
       </c>
-      <c r="C134" s="71" t="s">
+      <c r="D134" s="45" t="s">
         <v>81</v>
-      </c>
-      <c r="D134" s="45" t="s">
-        <v>82</v>
       </c>
       <c r="E134" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="135" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A135" s="78" t="s">
+      <c r="A135" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B135" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="C135" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="D135" s="45" t="s">
         <v>118</v>
-      </c>
-      <c r="C135" s="71" t="s">
-        <v>119</v>
-      </c>
-      <c r="D135" s="45" t="s">
-        <v>120</v>
       </c>
       <c r="E135" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="136" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A136" s="78" t="s">
+      <c r="A136" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B136" s="50" t="s">
+        <v>165</v>
+      </c>
+      <c r="C136" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="D136" s="45" t="s">
         <v>167</v>
-      </c>
-      <c r="C136" s="59" t="s">
-        <v>168</v>
-      </c>
-      <c r="D136" s="45" t="s">
-        <v>169</v>
       </c>
       <c r="E136" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="137" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A137" s="78" t="s">
+      <c r="A137" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B137" s="50" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C137" s="59" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D137" s="45" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E137" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="138" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A138" s="78" t="s">
+      <c r="A138" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B138" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="C138" s="71" t="s">
+        <v>106</v>
+      </c>
+      <c r="D138" s="45" t="s">
         <v>107</v>
-      </c>
-      <c r="C138" s="71" t="s">
-        <v>108</v>
-      </c>
-      <c r="D138" s="45" t="s">
-        <v>109</v>
       </c>
       <c r="E138" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="139" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A139" s="78" t="s">
+      <c r="A139" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B139" s="50" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C139" s="59" t="s">
         <v>59</v>
       </c>
       <c r="D139" s="45" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E139" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="140" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A140" s="78" t="s">
+      <c r="A140" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B140" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="C140" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="D140" s="45" t="s">
         <v>170</v>
-      </c>
-      <c r="C140" s="59" t="s">
-        <v>171</v>
-      </c>
-      <c r="D140" s="45" t="s">
-        <v>172</v>
       </c>
       <c r="E140" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="141" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A141" s="78" t="s">
+      <c r="A141" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B141" s="50" t="s">
+        <v>177</v>
+      </c>
+      <c r="C141" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="D141" s="45" t="s">
         <v>179</v>
-      </c>
-      <c r="C141" s="59" t="s">
-        <v>180</v>
-      </c>
-      <c r="D141" s="45" t="s">
-        <v>181</v>
       </c>
       <c r="E141" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="142" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A142" s="78" t="s">
+      <c r="A142" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B142" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C142" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="D142" s="45" t="s">
         <v>113</v>
-      </c>
-      <c r="C142" s="71" t="s">
-        <v>114</v>
-      </c>
-      <c r="D142" s="45" t="s">
-        <v>115</v>
       </c>
       <c r="E142" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="143" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A143" s="78" t="s">
+      <c r="A143" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B143" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="C143" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="D143" s="45" t="s">
         <v>164</v>
-      </c>
-      <c r="C143" s="59" t="s">
-        <v>165</v>
-      </c>
-      <c r="D143" s="45" t="s">
-        <v>166</v>
       </c>
       <c r="E143" s="48">
         <v>42664</v>
       </c>
     </row>
     <row r="144" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A144" s="78" t="s">
+      <c r="A144" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B144" s="49" t="s">
@@ -5102,7 +5109,7 @@
       </c>
     </row>
     <row r="145" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A145" s="78" t="s">
+      <c r="A145" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B145" s="49" t="s">
@@ -5112,216 +5119,216 @@
         <v>49</v>
       </c>
       <c r="D145" s="49" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E145" s="48">
         <v>42975</v>
       </c>
     </row>
     <row r="146" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A146" s="78" t="s">
+      <c r="A146" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B146" s="50" t="s">
         <v>55</v>
       </c>
       <c r="C146" s="71" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D146" s="45" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E146" s="48">
         <v>42975</v>
       </c>
     </row>
     <row r="147" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A147" s="78" t="s">
+      <c r="A147" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B147" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C147" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="C147" s="63" t="s">
+      <c r="D147" s="40" t="s">
         <v>87</v>
-      </c>
-      <c r="D147" s="40" t="s">
-        <v>88</v>
       </c>
       <c r="E147" s="48">
         <v>43037</v>
       </c>
     </row>
     <row r="148" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A148" s="78" t="s">
+      <c r="A148" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B148" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="C148" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="C148" s="71" t="s">
+      <c r="D148" s="45" t="s">
         <v>84</v>
-      </c>
-      <c r="D148" s="45" t="s">
-        <v>85</v>
       </c>
       <c r="E148" s="48">
         <v>43037</v>
       </c>
     </row>
     <row r="149" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A149" s="78" t="s">
+      <c r="A149" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B149" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="C149" s="59" t="s">
+        <v>217</v>
+      </c>
+      <c r="D149" s="45" t="s">
         <v>218</v>
-      </c>
-      <c r="C149" s="59" t="s">
-        <v>219</v>
-      </c>
-      <c r="D149" s="45" t="s">
-        <v>220</v>
       </c>
       <c r="E149" s="48">
         <v>43296</v>
       </c>
     </row>
     <row r="150" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A150" s="78" t="s">
+      <c r="A150" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B150" s="50" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C150" s="59" t="s">
         <v>57</v>
       </c>
       <c r="D150" s="45" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E150" s="48">
         <v>43296</v>
       </c>
     </row>
     <row r="151" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A151" s="78" t="s">
+      <c r="A151" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B151" s="50" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C151" s="59" t="s">
         <v>57</v>
       </c>
       <c r="D151" s="45" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E151" s="48">
         <v>43296</v>
       </c>
     </row>
     <row r="152" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A152" s="78" t="s">
+      <c r="A152" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B152" s="50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C152" s="59" t="s">
         <v>66</v>
       </c>
       <c r="D152" s="45" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E152" s="48">
         <v>43588</v>
       </c>
     </row>
     <row r="153" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A153" s="78" t="s">
+      <c r="A153" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B153" s="49" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C153" s="62" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D153" s="49" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E153" s="48">
         <v>43588</v>
       </c>
     </row>
     <row r="154" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A154" s="78" t="s">
+      <c r="A154" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B154" s="50" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C154" s="59" t="s">
         <v>63</v>
       </c>
       <c r="D154" s="45" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E154" s="48">
         <v>43861</v>
       </c>
     </row>
     <row r="155" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A155" s="78" t="s">
+      <c r="A155" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B155" s="50" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C155" s="59" t="s">
         <v>63</v>
       </c>
       <c r="D155" s="45" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E155" s="48">
         <v>43861</v>
       </c>
     </row>
     <row r="156" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A156" s="78" t="s">
+      <c r="A156" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B156" s="49" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C156" s="63" t="s">
         <v>63</v>
       </c>
       <c r="D156" s="49" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E156" s="48">
         <v>43861</v>
       </c>
     </row>
     <row r="157" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A157" s="78" t="s">
+      <c r="A157" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B157" s="50" t="s">
         <v>51</v>
       </c>
       <c r="C157" s="71" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="D157" s="45" t="s">
-        <v>71</v>
+        <v>327</v>
       </c>
       <c r="E157" s="48"/>
     </row>
     <row r="158" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A158" s="78" t="s">
+      <c r="A158" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B158" s="50" t="s">
@@ -5331,87 +5338,87 @@
         <v>49</v>
       </c>
       <c r="D158" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E158" s="48"/>
     </row>
     <row r="159" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="76" t="s">
+      <c r="A159" s="75" t="s">
         <v>3</v>
       </c>
       <c r="B159" s="40" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C159" s="63" t="s">
         <v>62</v>
       </c>
       <c r="D159" s="45" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="E159" s="54"/>
     </row>
     <row r="160" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A160" s="78" t="s">
+      <c r="A160" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B160" s="40" t="s">
         <v>52</v>
       </c>
       <c r="C160" s="63" t="s">
-        <v>93</v>
+        <v>346</v>
       </c>
       <c r="D160" s="45" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E160" s="48"/>
     </row>
     <row r="161" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A161" s="78" t="s">
+      <c r="A161" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B161" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C161" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="C161" s="63" t="s">
+      <c r="D161" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="D161" s="49" t="s">
-        <v>92</v>
-      </c>
       <c r="E161" s="48"/>
     </row>
     <row r="162" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A162" s="76" t="s">
+      <c r="A162" s="75" t="s">
         <v>3</v>
       </c>
       <c r="B162" s="40" t="s">
-        <v>327</v>
+        <v>345</v>
       </c>
       <c r="C162" s="71" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D162" s="45" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="E162" s="48"/>
     </row>
     <row r="163" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A163" s="76" t="s">
+      <c r="A163" s="75" t="s">
         <v>8</v>
       </c>
       <c r="B163" s="50" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C163" s="50" t="s">
+        <v>316</v>
+      </c>
+      <c r="D163" s="45" t="s">
         <v>318</v>
       </c>
-      <c r="D163" s="45" t="s">
-        <v>320</v>
-      </c>
       <c r="E163" s="48"/>
     </row>
     <row r="164" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A164" s="78" t="s">
+      <c r="A164" s="77" t="s">
         <v>3</v>
       </c>
       <c r="B164" s="50" t="s">
@@ -5426,172 +5433,172 @@
       <c r="E164" s="48"/>
     </row>
     <row r="165" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A165" s="76" t="s">
+      <c r="A165" s="75" t="s">
         <v>3</v>
       </c>
       <c r="B165" s="40" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C165" s="55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D165" s="45" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="E165" s="48"/>
     </row>
     <row r="166" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A166" s="76" t="s">
+      <c r="A166" s="75" t="s">
         <v>8</v>
       </c>
       <c r="B166" s="40" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="C166" s="40" t="s">
-        <v>322</v>
+        <v>347</v>
       </c>
       <c r="D166" s="45" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E166" s="48"/>
     </row>
     <row r="167" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="76" t="s">
+      <c r="A167" s="75" t="s">
         <v>3</v>
       </c>
       <c r="B167" s="40" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C167" s="40" t="s">
         <v>62</v>
       </c>
       <c r="D167" s="45" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E167" s="54"/>
     </row>
     <row r="168" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A168" s="76" t="s">
+      <c r="A168" s="75" t="s">
         <v>3</v>
       </c>
       <c r="B168" s="40" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C168" s="50" t="s">
         <v>49</v>
       </c>
       <c r="D168" s="45" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="E168" s="48"/>
     </row>
     <row r="169" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A169" s="78" t="s">
+      <c r="A169" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B169" s="50" t="s">
+        <v>205</v>
+      </c>
+      <c r="C169" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="D169" s="45" t="s">
         <v>207</v>
       </c>
-      <c r="C169" s="50" t="s">
-        <v>208</v>
-      </c>
-      <c r="D169" s="45" t="s">
-        <v>209</v>
-      </c>
       <c r="E169" s="48"/>
     </row>
     <row r="170" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="76" t="s">
+      <c r="A170" s="75" t="s">
         <v>3</v>
       </c>
       <c r="B170" s="40" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C170" s="40" t="s">
         <v>62</v>
       </c>
       <c r="D170" s="45" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="E170" s="54"/>
     </row>
     <row r="171" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A171" s="76" t="s">
+      <c r="A171" s="75" t="s">
         <v>8</v>
       </c>
       <c r="B171" s="40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C171" s="40" t="s">
         <v>49</v>
       </c>
       <c r="D171" s="40" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E171" s="48"/>
     </row>
     <row r="172" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A172" s="78" t="s">
+      <c r="A172" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B172" s="50" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C172" s="50" t="s">
         <v>49</v>
       </c>
       <c r="D172" s="45" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E172" s="48"/>
     </row>
     <row r="173" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A173" s="78" t="s">
+      <c r="A173" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B173" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C173" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="D173" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C173" s="50" t="s">
-        <v>98</v>
-      </c>
-      <c r="D173" s="45" t="s">
-        <v>99</v>
-      </c>
       <c r="E173" s="48"/>
     </row>
     <row r="174" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="76" t="s">
+      <c r="A174" s="75" t="s">
         <v>3</v>
       </c>
       <c r="B174" s="40" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C174" s="40" t="s">
         <v>62</v>
       </c>
       <c r="D174" s="45" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E174" s="60"/>
     </row>
     <row r="175" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A175" s="76" t="s">
+      <c r="A175" s="75" t="s">
         <v>8</v>
       </c>
       <c r="B175" s="40" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C175" s="50" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D175" s="45" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E175" s="67"/>
     </row>
     <row r="176" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A176" s="78" t="s">
+      <c r="A176" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B176" s="49" t="s">
@@ -5601,59 +5608,59 @@
         <v>49</v>
       </c>
       <c r="D176" s="49" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E176" s="67"/>
     </row>
     <row r="177" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A177" s="76" t="s">
+      <c r="A177" s="75" t="s">
         <v>8</v>
       </c>
       <c r="B177" s="50" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="C177" s="50" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D177" s="45" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E177" s="67"/>
     </row>
     <row r="178" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="76" t="s">
+      <c r="A178" s="75" t="s">
         <v>3</v>
       </c>
       <c r="B178" s="40" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="C178" s="40" t="s">
         <v>62</v>
       </c>
       <c r="D178" s="45" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E178" s="60"/>
     </row>
     <row r="179" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A179" s="76"/>
+      <c r="A179" s="75"/>
       <c r="B179" s="40"/>
       <c r="C179" s="40"/>
       <c r="D179" s="45"/>
       <c r="E179" s="60"/>
     </row>
     <row r="180" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A180" s="76"/>
+      <c r="A180" s="75"/>
       <c r="B180" s="40"/>
       <c r="C180" s="40"/>
       <c r="D180" s="45"/>
       <c r="E180" s="60"/>
     </row>
     <row r="181" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A181" s="76"/>
+      <c r="A181" s="75"/>
       <c r="B181" s="44"/>
       <c r="C181" s="44"/>
-      <c r="D181" s="75"/>
+      <c r="D181" s="74"/>
       <c r="E181" s="65"/>
     </row>
     <row r="182" spans="1:5" s="34" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -5664,13 +5671,13 @@
       <c r="E182" s="9"/>
     </row>
     <row r="183" spans="1:5" s="34" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A183" s="86" t="s">
+      <c r="A183" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="B183" s="86"/>
-      <c r="C183" s="86"/>
-      <c r="D183" s="86"/>
-      <c r="E183" s="86"/>
+      <c r="B183" s="85"/>
+      <c r="C183" s="85"/>
+      <c r="D183" s="85"/>
+      <c r="E183" s="85"/>
     </row>
     <row r="184" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A184" s="34" t="s">
@@ -5717,17 +5724,17 @@
       </c>
     </row>
     <row r="188" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A188" s="76" t="s">
+      <c r="A188" s="75" t="s">
         <v>10</v>
       </c>
       <c r="B188" s="40" t="s">
+        <v>312</v>
+      </c>
+      <c r="C188" s="40" t="s">
+        <v>313</v>
+      </c>
+      <c r="D188" s="40" t="s">
         <v>314</v>
-      </c>
-      <c r="C188" s="40" t="s">
-        <v>315</v>
-      </c>
-      <c r="D188" s="40" t="s">
-        <v>316</v>
       </c>
       <c r="E188" s="60">
         <v>43293</v>
@@ -5737,64 +5744,64 @@
       <c r="A189" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B189" s="44" t="s">
-        <v>324</v>
-      </c>
-      <c r="C189" s="44" t="s">
-        <v>326</v>
-      </c>
-      <c r="D189" s="75" t="s">
-        <v>325</v>
-      </c>
-      <c r="E189" s="60"/>
+      <c r="B189" s="64" t="s">
+        <v>310</v>
+      </c>
+      <c r="C189" s="64" t="s">
+        <v>309</v>
+      </c>
+      <c r="D189" s="92" t="s">
+        <v>311</v>
+      </c>
+      <c r="E189" s="67"/>
     </row>
     <row r="190" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A190" s="52" t="s">
+      <c r="A190" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="B190" s="53" t="s">
-        <v>312</v>
-      </c>
-      <c r="C190" s="53" t="s">
-        <v>311</v>
+      <c r="B190" s="55" t="s">
+        <v>306</v>
+      </c>
+      <c r="C190" s="91" t="s">
+        <v>307</v>
       </c>
       <c r="D190" s="56" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="E190" s="48"/>
     </row>
     <row r="191" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A191" s="77" t="s">
+      <c r="A191" s="76" t="s">
         <v>4</v>
       </c>
       <c r="B191" s="55" t="s">
-        <v>308</v>
-      </c>
-      <c r="C191" s="74" t="s">
-        <v>309</v>
-      </c>
-      <c r="D191" s="56" t="s">
-        <v>310</v>
+        <v>303</v>
+      </c>
+      <c r="C191" s="44" t="s">
+        <v>304</v>
+      </c>
+      <c r="D191" s="55" t="s">
+        <v>305</v>
       </c>
       <c r="E191" s="48"/>
     </row>
     <row r="192" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A192" s="78" t="s">
+      <c r="A192" s="77" t="s">
         <v>4</v>
       </c>
       <c r="B192" s="40" t="s">
-        <v>305</v>
+        <v>344</v>
       </c>
       <c r="C192" s="55" t="s">
-        <v>306</v>
-      </c>
-      <c r="D192" s="40" t="s">
-        <v>307</v>
-      </c>
-      <c r="E192" s="67"/>
+        <v>322</v>
+      </c>
+      <c r="D192" s="93" t="s">
+        <v>321</v>
+      </c>
+      <c r="E192" s="60"/>
     </row>
     <row r="193" spans="1:5" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A193" s="78"/>
+      <c r="A193" s="77"/>
       <c r="B193" s="40"/>
       <c r="C193" s="40"/>
       <c r="D193" s="45"/>
@@ -5975,7 +5982,7 @@
     <hyperlink ref="D163" r:id="rId3" xr:uid="{75A57B4F-5516-424E-B243-D3B13A1DCB71}"/>
     <hyperlink ref="D175" r:id="rId4" xr:uid="{D4087D8D-2388-6E41-92AC-15178D54BEC9}"/>
     <hyperlink ref="D166" r:id="rId5" xr:uid="{362C7F51-29E4-CC40-A0C6-5C9D4C1827D6}"/>
-    <hyperlink ref="D189" r:id="rId6" xr:uid="{14152F92-F184-294C-B3DF-EBB3F8C4169B}"/>
+    <hyperlink ref="D192" r:id="rId6" xr:uid="{14152F92-F184-294C-B3DF-EBB3F8C4169B}"/>
     <hyperlink ref="D162" r:id="rId7" xr:uid="{04B042A6-4EE8-7642-AEED-608BB942C487}"/>
     <hyperlink ref="D168" r:id="rId8" xr:uid="{53AEA3C2-0239-594F-BDE2-735D71A81616}"/>
     <hyperlink ref="D165" r:id="rId9" xr:uid="{24D20773-A046-324F-A608-336E473D3959}"/>
@@ -5984,15 +5991,16 @@
     <hyperlink ref="D174" r:id="rId12" xr:uid="{E8D86930-5BCF-234D-A742-6D3175BADFC8}"/>
     <hyperlink ref="D170" r:id="rId13" xr:uid="{3FD28ED8-2162-8247-A1AB-3B1641CE3960}"/>
     <hyperlink ref="D159" r:id="rId14" xr:uid="{8694CD59-5D54-DC41-8308-2A7826D74C21}"/>
+    <hyperlink ref="D157" r:id="rId15" xr:uid="{FE08D58B-810E-5A49-ACC3-B7013951D3D2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="98" fitToHeight="0" orientation="portrait" r:id="rId15"/>
+  <pageSetup scale="98" fitToHeight="0" orientation="portrait" r:id="rId16"/>
   <tableParts count="5">
-    <tablePart r:id="rId16"/>
     <tablePart r:id="rId17"/>
     <tablePart r:id="rId18"/>
     <tablePart r:id="rId19"/>
     <tablePart r:id="rId20"/>
+    <tablePart r:id="rId21"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>